<commit_message>
1 camada best 70 neuronios
</commit_message>
<xml_diff>
--- a/nuno-dataset/test-solidos-02/better_results.xlsx
+++ b/nuno-dataset/test-solidos-02/better_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,898 +487,742 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>model_6_7_7</t>
+          <t>model_14_5_14</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.9234879187990968</v>
+        <v>0.793455378695981</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8457773776739879</v>
+        <v>0.4244238555107573</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8545100641925611</v>
+        <v>0.6608014781599317</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8620567393958509</v>
+        <v>0.5678008674674568</v>
       </c>
       <c r="G2" t="n">
-        <v>9.22737979888916</v>
+        <v>24.90934371948242</v>
       </c>
       <c r="H2" t="n">
-        <v>12.42074298858643</v>
+        <v>81.53942108154297</v>
       </c>
       <c r="I2" t="n">
-        <v>6.698015689849854</v>
+        <v>57.88400268554688</v>
       </c>
       <c r="J2" t="n">
-        <v>9.727782249450684</v>
+        <v>70.40745544433594</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Hidden Size=[30, 25], regularizer=0.1, learning_rate=0.02</t>
+          <t>Hidden Size=[70], regularizer=0.1, learning_rate=0.02</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>model_6_7_6</t>
+          <t>model_14_5_13</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.9225063257008925</v>
+        <v>0.7933326582680003</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8526547412917236</v>
+        <v>0.4251372654216189</v>
       </c>
       <c r="E3" t="n">
-        <v>0.862965961353646</v>
+        <v>0.6617347785971694</v>
       </c>
       <c r="F3" t="n">
-        <v>0.868813424944812</v>
+        <v>0.5685893796917934</v>
       </c>
       <c r="G3" t="n">
-        <v>9.345759391784668</v>
+        <v>24.92414283752441</v>
       </c>
       <c r="H3" t="n">
-        <v>11.86685562133789</v>
+        <v>81.43834686279297</v>
       </c>
       <c r="I3" t="n">
-        <v>6.308725833892822</v>
+        <v>57.72473907470703</v>
       </c>
       <c r="J3" t="n">
-        <v>9.251297950744629</v>
+        <v>70.27899932861328</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Hidden Size=[30, 25], regularizer=0.1, learning_rate=0.02</t>
+          <t>Hidden Size=[70], regularizer=0.1, learning_rate=0.02</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>model_6_6_4</t>
+          <t>model_14_5_15</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.8854880312727619</v>
+        <v>0.7926857422892021</v>
       </c>
       <c r="D4" t="n">
-        <v>0.974398169535678</v>
+        <v>0.4208282591181479</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8692711020061304</v>
+        <v>0.6596114599989675</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9342991117803169</v>
+        <v>0.5655588562216785</v>
       </c>
       <c r="G4" t="n">
-        <v>13.81017780303955</v>
+        <v>25.00216102600098</v>
       </c>
       <c r="H4" t="n">
-        <v>3.851471424102783</v>
+        <v>82.04879760742188</v>
       </c>
       <c r="I4" t="n">
-        <v>14.17279529571533</v>
+        <v>58.08708190917969</v>
       </c>
       <c r="J4" t="n">
-        <v>8.708565711975098</v>
+        <v>70.77268981933594</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Hidden Size=[30, 25], regularizer=0.1, learning_rate=0.02</t>
+          <t>Hidden Size=[70], regularizer=0.1, learning_rate=0.02</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>model_6_6_5</t>
+          <t>model_14_5_16</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.8850855583404778</v>
+        <v>0.7926851762345462</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9678731674407923</v>
+        <v>0.4125075173457247</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8476522546703948</v>
+        <v>0.6562808351878726</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9220573569962218</v>
+        <v>0.5600862037542027</v>
       </c>
       <c r="G5" t="n">
-        <v>13.85871601104736</v>
+        <v>25.00222969055176</v>
       </c>
       <c r="H5" t="n">
-        <v>4.833075523376465</v>
+        <v>83.22755432128906</v>
       </c>
       <c r="I5" t="n">
-        <v>16.51657295227051</v>
+        <v>58.65545272827148</v>
       </c>
       <c r="J5" t="n">
-        <v>10.3311939239502</v>
+        <v>71.66421508789062</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Hidden Size=[30, 25], regularizer=0.1, learning_rate=0.02</t>
+          <t>Hidden Size=[70], regularizer=0.1, learning_rate=0.02</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>model_6_6_3</t>
+          <t>model_14_5_11</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.8837427699794401</v>
+        <v>0.7926035815570951</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9791903513174703</v>
+        <v>0.4327968716939861</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8788294884746145</v>
+        <v>0.6700305331880225</v>
       </c>
       <c r="F6" t="n">
-        <v>0.94085757387903</v>
+        <v>0.5762051655466813</v>
       </c>
       <c r="G6" t="n">
-        <v>14.02065563201904</v>
+        <v>25.0120677947998</v>
       </c>
       <c r="H6" t="n">
-        <v>3.130548238754272</v>
+        <v>80.35324859619141</v>
       </c>
       <c r="I6" t="n">
-        <v>13.13653564453125</v>
+        <v>56.30907440185547</v>
       </c>
       <c r="J6" t="n">
-        <v>7.839249610900879</v>
+        <v>69.03835296630859</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Hidden Size=[30, 25], regularizer=0.1, learning_rate=0.02</t>
+          <t>Hidden Size=[70], regularizer=0.1, learning_rate=0.02</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>model_6_6_6</t>
+          <t>model_14_5_12</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.8823248011093614</v>
+        <v>0.7924749114419452</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9608470341107334</v>
+        <v>0.4250480315879348</v>
       </c>
       <c r="E7" t="n">
-        <v>0.8094127451722819</v>
+        <v>0.6610854657107283</v>
       </c>
       <c r="F7" t="n">
-        <v>0.9031170968213512</v>
+        <v>0.5682281144890153</v>
       </c>
       <c r="G7" t="n">
-        <v>14.19166374206543</v>
+        <v>25.027587890625</v>
       </c>
       <c r="H7" t="n">
-        <v>5.890068531036377</v>
+        <v>81.45098876953125</v>
       </c>
       <c r="I7" t="n">
-        <v>20.66225814819336</v>
+        <v>57.83554458618164</v>
       </c>
       <c r="J7" t="n">
-        <v>12.84169960021973</v>
+        <v>70.33785247802734</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Hidden Size=[30, 25], regularizer=0.1, learning_rate=0.02</t>
+          <t>Hidden Size=[70], regularizer=0.1, learning_rate=0.02</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>model_6_6_2</t>
+          <t>model_14_5_17</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.8805670726392637</v>
+        <v>0.7917328975520058</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9822572623160387</v>
+        <v>0.4085525486840363</v>
       </c>
       <c r="E8" t="n">
-        <v>0.8819989140249673</v>
+        <v>0.6530655525354701</v>
       </c>
       <c r="F8" t="n">
-        <v>0.9439203009188547</v>
+        <v>0.5566803899427601</v>
       </c>
       <c r="G8" t="n">
-        <v>14.40364646911621</v>
+        <v>25.11707496643066</v>
       </c>
       <c r="H8" t="n">
-        <v>2.669170379638672</v>
+        <v>83.78783416748047</v>
       </c>
       <c r="I8" t="n">
-        <v>12.79292774200439</v>
+        <v>59.20413589477539</v>
       </c>
       <c r="J8" t="n">
-        <v>7.433289527893066</v>
+        <v>72.21903991699219</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Hidden Size=[30, 25], regularizer=0.1, learning_rate=0.02</t>
+          <t>Hidden Size=[70], regularizer=0.1, learning_rate=0.02</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>model_6_6_1</t>
+          <t>model_14_5_10</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.877040569723336</v>
+        <v>0.7909776258259271</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9835499036138331</v>
+        <v>0.4349555093314732</v>
       </c>
       <c r="E9" t="n">
-        <v>0.8847351208431866</v>
+        <v>0.6747804025417153</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9457501212811317</v>
+        <v>0.5795405364507769</v>
       </c>
       <c r="G9" t="n">
-        <v>14.82894325256348</v>
+        <v>25.20816040039062</v>
       </c>
       <c r="H9" t="n">
-        <v>2.474708795547485</v>
+        <v>80.04744720458984</v>
       </c>
       <c r="I9" t="n">
-        <v>12.4962854385376</v>
+        <v>55.49851226806641</v>
       </c>
       <c r="J9" t="n">
-        <v>7.190749168395996</v>
+        <v>68.49500274658203</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Hidden Size=[30, 25], regularizer=0.1, learning_rate=0.02</t>
+          <t>Hidden Size=[70], regularizer=0.1, learning_rate=0.02</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>model_6_6_7</t>
+          <t>model_14_5_18</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.8769513076390688</v>
+        <v>0.7906625088001537</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9523434373709323</v>
+        <v>0.397027494809812</v>
       </c>
       <c r="E10" t="n">
-        <v>0.7529408388755892</v>
+        <v>0.6469965126492243</v>
       </c>
       <c r="F10" t="n">
-        <v>0.8762716110791339</v>
+        <v>0.5483825932525763</v>
       </c>
       <c r="G10" t="n">
-        <v>14.83970832824707</v>
+        <v>25.24616432189941</v>
       </c>
       <c r="H10" t="n">
-        <v>7.169326782226562</v>
+        <v>85.42054748535156</v>
       </c>
       <c r="I10" t="n">
-        <v>26.78458213806152</v>
+        <v>60.23981475830078</v>
       </c>
       <c r="J10" t="n">
-        <v>16.40003395080566</v>
+        <v>73.57079315185547</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Hidden Size=[30, 25], regularizer=0.1, learning_rate=0.02</t>
+          <t>Hidden Size=[70], regularizer=0.1, learning_rate=0.02</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>model_6_6_0</t>
+          <t>model_14_5_19</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.8730924512031406</v>
+        <v>0.7903474439790713</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9840570892765397</v>
+        <v>0.3944160967622141</v>
       </c>
       <c r="E11" t="n">
-        <v>0.8867896597161887</v>
+        <v>0.6467230160030752</v>
       </c>
       <c r="F11" t="n">
-        <v>0.946845701607713</v>
+        <v>0.5470455344634841</v>
       </c>
       <c r="G11" t="n">
-        <v>15.30508899688721</v>
+        <v>25.28416061401367</v>
       </c>
       <c r="H11" t="n">
-        <v>2.398409366607666</v>
+        <v>85.79049682617188</v>
       </c>
       <c r="I11" t="n">
-        <v>12.27354526519775</v>
+        <v>60.28648376464844</v>
       </c>
       <c r="J11" t="n">
-        <v>7.045531749725342</v>
+        <v>73.78861236572266</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Hidden Size=[30, 25], regularizer=0.1, learning_rate=0.02</t>
+          <t>Hidden Size=[70], regularizer=0.1, learning_rate=0.02</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>model_6_6_8</t>
+          <t>model_14_5_20</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.869329973454215</v>
+        <v>0.7889205318091564</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9445719632634457</v>
+        <v>0.3841195382909653</v>
       </c>
       <c r="E12" t="n">
-        <v>0.6796142988125431</v>
+        <v>0.6447578324635511</v>
       </c>
       <c r="F12" t="n">
-        <v>0.843378536095339</v>
+        <v>0.5413363867777254</v>
       </c>
       <c r="G12" t="n">
-        <v>15.75884437561035</v>
+        <v>25.45624923706055</v>
       </c>
       <c r="H12" t="n">
-        <v>8.338446617126465</v>
+        <v>87.24916076660156</v>
       </c>
       <c r="I12" t="n">
-        <v>34.73418426513672</v>
+        <v>60.62184143066406</v>
       </c>
       <c r="J12" t="n">
-        <v>20.75996589660645</v>
+        <v>74.71865844726562</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Hidden Size=[30, 25], regularizer=0.1, learning_rate=0.02</t>
+          <t>Hidden Size=[70], regularizer=0.1, learning_rate=0.02</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>model_6_5_24</t>
+          <t>model_14_5_21</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.8688111845797573</v>
+        <v>0.7879561570013363</v>
       </c>
       <c r="D13" t="n">
-        <v>0.6688424715801964</v>
+        <v>0.3771577554230655</v>
       </c>
       <c r="E13" t="n">
-        <v>0.6302994269434514</v>
+        <v>0.6438289684487419</v>
       </c>
       <c r="F13" t="n">
-        <v>0.6979718412449025</v>
+        <v>0.537673397975859</v>
       </c>
       <c r="G13" t="n">
-        <v>15.8214111328125</v>
+        <v>25.57254981994629</v>
       </c>
       <c r="H13" t="n">
-        <v>25.63688087463379</v>
+        <v>88.23540496826172</v>
       </c>
       <c r="I13" t="n">
-        <v>41.94471740722656</v>
+        <v>60.78035736083984</v>
       </c>
       <c r="J13" t="n">
-        <v>33.31114959716797</v>
+        <v>75.31536865234375</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Hidden Size=[30, 25], regularizer=0.1, learning_rate=0.02</t>
+          <t>Hidden Size=[70], regularizer=0.1, learning_rate=0.02</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>model_6_5_23</t>
+          <t>model_14_5_22</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.8681320669197793</v>
+        <v>0.7871192185515063</v>
       </c>
       <c r="D14" t="n">
-        <v>0.6652419562727336</v>
+        <v>0.3732352104046813</v>
       </c>
       <c r="E14" t="n">
-        <v>0.6420125266462886</v>
+        <v>0.6430237927975164</v>
       </c>
       <c r="F14" t="n">
-        <v>0.7023039006069022</v>
+        <v>0.5354705409969531</v>
       </c>
       <c r="G14" t="n">
-        <v>15.90331172943115</v>
+        <v>25.67348289489746</v>
       </c>
       <c r="H14" t="n">
-        <v>25.91561889648438</v>
+        <v>88.79109191894531</v>
       </c>
       <c r="I14" t="n">
-        <v>40.61579132080078</v>
+        <v>60.91775512695312</v>
       </c>
       <c r="J14" t="n">
-        <v>32.83335876464844</v>
+        <v>75.67423248291016</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Hidden Size=[30, 25], regularizer=0.1, learning_rate=0.02</t>
+          <t>Hidden Size=[70], regularizer=0.1, learning_rate=0.02</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>model_6_5_22</t>
+          <t>model_14_5_9</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.8613212693283038</v>
+        <v>0.7849273560535748</v>
       </c>
       <c r="D15" t="n">
-        <v>0.6252492934464045</v>
+        <v>0.42143929759103</v>
       </c>
       <c r="E15" t="n">
-        <v>0.6412490630199101</v>
+        <v>0.6863836637931482</v>
       </c>
       <c r="F15" t="n">
-        <v>0.6870729068711843</v>
+        <v>0.5790378269812004</v>
       </c>
       <c r="G15" t="n">
-        <v>16.72469711303711</v>
+        <v>25.93782424926758</v>
       </c>
       <c r="H15" t="n">
-        <v>29.01168823242188</v>
+        <v>81.96223449707031</v>
       </c>
       <c r="I15" t="n">
-        <v>40.70241546630859</v>
+        <v>53.51842498779297</v>
       </c>
       <c r="J15" t="n">
-        <v>34.51321411132812</v>
+        <v>68.57689666748047</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Hidden Size=[30, 25], regularizer=0.1, learning_rate=0.02</t>
+          <t>Hidden Size=[70], regularizer=0.1, learning_rate=0.02</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>model_6_5_21</t>
+          <t>model_14_5_8</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.8594091903203452</v>
+        <v>0.7820880988355638</v>
       </c>
       <c r="D16" t="n">
-        <v>0.6149787807294418</v>
+        <v>0.4299180728352087</v>
       </c>
       <c r="E16" t="n">
-        <v>0.6500010302477016</v>
+        <v>0.6949359057733493</v>
       </c>
       <c r="F16" t="n">
-        <v>0.6874932120125538</v>
+        <v>0.5871571571626681</v>
       </c>
       <c r="G16" t="n">
-        <v>16.95529365539551</v>
+        <v>26.28023910522461</v>
       </c>
       <c r="H16" t="n">
-        <v>29.80679321289062</v>
+        <v>80.76107788085938</v>
       </c>
       <c r="I16" t="n">
-        <v>39.70944976806641</v>
+        <v>52.05898666381836</v>
       </c>
       <c r="J16" t="n">
-        <v>34.46685409545898</v>
+        <v>67.25421142578125</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Hidden Size=[30, 25], regularizer=0.1, learning_rate=0.02</t>
+          <t>Hidden Size=[70], regularizer=0.1, learning_rate=0.02</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>model_6_5_20</t>
+          <t>model_14_5_7</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.8574600930498262</v>
+        <v>0.7722166036937503</v>
       </c>
       <c r="D17" t="n">
-        <v>0.6044126338120748</v>
+        <v>0.4088311356072766</v>
       </c>
       <c r="E17" t="n">
-        <v>0.6610122633608817</v>
+        <v>0.7188197538103283</v>
       </c>
       <c r="F17" t="n">
-        <v>0.6888968383346321</v>
+        <v>0.5892227943444696</v>
       </c>
       <c r="G17" t="n">
-        <v>17.19035530090332</v>
+        <v>27.47074317932129</v>
       </c>
       <c r="H17" t="n">
-        <v>30.62477874755859</v>
+        <v>83.74837493896484</v>
       </c>
       <c r="I17" t="n">
-        <v>38.46015930175781</v>
+        <v>47.98322296142578</v>
       </c>
       <c r="J17" t="n">
-        <v>34.31204605102539</v>
+        <v>66.91771697998047</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Hidden Size=[30, 25], regularizer=0.1, learning_rate=0.02</t>
+          <t>Hidden Size=[70], regularizer=0.1, learning_rate=0.02</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>model_6_5_19</t>
+          <t>model_14_5_5</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.855015451225256</v>
+        <v>0.7704571756280686</v>
       </c>
       <c r="D18" t="n">
-        <v>0.5907565419894633</v>
+        <v>0.474431173880703</v>
       </c>
       <c r="E18" t="n">
-        <v>0.6714532368637556</v>
+        <v>0.7483886158846897</v>
       </c>
       <c r="F18" t="n">
-        <v>0.6888770537549194</v>
+        <v>0.6340003993584564</v>
       </c>
       <c r="G18" t="n">
-        <v>17.48517990112305</v>
+        <v>27.68293190002441</v>
       </c>
       <c r="H18" t="n">
-        <v>31.68198013305664</v>
+        <v>74.45509338378906</v>
       </c>
       <c r="I18" t="n">
-        <v>37.27556991577148</v>
+        <v>42.93731689453125</v>
       </c>
       <c r="J18" t="n">
-        <v>34.31422805786133</v>
+        <v>59.62321472167969</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Hidden Size=[30, 25], regularizer=0.1, learning_rate=0.02</t>
+          <t>Hidden Size=[70], regularizer=0.1, learning_rate=0.02</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>model_6_7_5</t>
+          <t>model_14_5_6</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.8546669284577366</v>
+        <v>0.7684996735102603</v>
       </c>
       <c r="D19" t="n">
-        <v>0.7808214822816034</v>
+        <v>0.4285630700220719</v>
       </c>
       <c r="E19" t="n">
-        <v>0.5328916584102521</v>
+        <v>0.7326629457130962</v>
       </c>
       <c r="F19" t="n">
-        <v>0.723978972061383</v>
+        <v>0.6051312181445232</v>
       </c>
       <c r="G19" t="n">
-        <v>17.52721214294434</v>
+        <v>27.91900825500488</v>
       </c>
       <c r="H19" t="n">
-        <v>17.65214347839355</v>
+        <v>80.95303344726562</v>
       </c>
       <c r="I19" t="n">
-        <v>21.50457382202148</v>
+        <v>45.62089538574219</v>
       </c>
       <c r="J19" t="n">
-        <v>19.46504592895508</v>
+        <v>64.32614898681641</v>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Hidden Size=[30, 25], regularizer=0.1, learning_rate=0.02</t>
+          <t>Hidden Size=[70], regularizer=0.1, learning_rate=0.02</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>model_6_7_4</t>
+          <t>model_13_5_0</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.8533291787823747</v>
+        <v>0.7642749634634054</v>
       </c>
       <c r="D20" t="n">
-        <v>0.7844868793709974</v>
+        <v>0.7044608375173393</v>
       </c>
       <c r="E20" t="n">
-        <v>0.5730483471873971</v>
+        <v>0.7791132756559503</v>
       </c>
       <c r="F20" t="n">
-        <v>0.7385317798578355</v>
+        <v>0.7271868847138594</v>
       </c>
       <c r="G20" t="n">
-        <v>17.68854331970215</v>
+        <v>28.42851066589355</v>
       </c>
       <c r="H20" t="n">
-        <v>17.35694122314453</v>
+        <v>60.08975601196289</v>
       </c>
       <c r="I20" t="n">
-        <v>19.65585327148438</v>
+        <v>22.10588073730469</v>
       </c>
       <c r="J20" t="n">
-        <v>18.43878173828125</v>
+        <v>42.21499633789062</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Hidden Size=[30, 25], regularizer=0.1, learning_rate=0.02</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>62</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>model_6_7_3</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>0.8510421778486663</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0.7885501299129154</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0.5989298370105036</v>
-      </c>
-      <c r="F21" t="n">
-        <v>0.7489395225530689</v>
-      </c>
-      <c r="G21" t="n">
-        <v>17.96435737609863</v>
-      </c>
-      <c r="H21" t="n">
-        <v>17.02969932556152</v>
-      </c>
-      <c r="I21" t="n">
-        <v>18.46432876586914</v>
-      </c>
-      <c r="J21" t="n">
-        <v>17.70482444763184</v>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>Hidden Size=[30, 25], regularizer=0.1, learning_rate=0.02</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>63</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>model_6_7_2</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>0.8495575540468232</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0.7998827119372898</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0.6287567700380059</v>
-      </c>
-      <c r="F22" t="n">
-        <v>0.7649545343617352</v>
-      </c>
-      <c r="G22" t="n">
-        <v>18.14340400695801</v>
-      </c>
-      <c r="H22" t="n">
-        <v>16.11699676513672</v>
-      </c>
-      <c r="I22" t="n">
-        <v>17.09116744995117</v>
-      </c>
-      <c r="J22" t="n">
-        <v>16.5754451751709</v>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>Hidden Size=[30, 25], regularizer=0.1, learning_rate=0.02</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>model_6_7_1</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>0.8481000732984031</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0.8121723741045487</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0.6601465026537429</v>
-      </c>
-      <c r="F23" t="n">
-        <v>0.782028555309924</v>
-      </c>
-      <c r="G23" t="n">
-        <v>18.31917381286621</v>
-      </c>
-      <c r="H23" t="n">
-        <v>15.12721633911133</v>
-      </c>
-      <c r="I23" t="n">
-        <v>15.64605808258057</v>
-      </c>
-      <c r="J23" t="n">
-        <v>15.37138080596924</v>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>Hidden Size=[30, 25], regularizer=0.1, learning_rate=0.02</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>67</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>model_6_7_0</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>0.8464792470016187</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0.8224049354601757</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0.6962610368356907</v>
-      </c>
-      <c r="F24" t="n">
-        <v>0.7993102168711836</v>
-      </c>
-      <c r="G24" t="n">
-        <v>18.5146484375</v>
-      </c>
-      <c r="H24" t="n">
-        <v>14.30310726165771</v>
-      </c>
-      <c r="I24" t="n">
-        <v>13.98342895507812</v>
-      </c>
-      <c r="J24" t="n">
-        <v>14.15267562866211</v>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>Hidden Size=[30, 25], regularizer=0.1, learning_rate=0.02</t>
+          <t>Hidden Size=[80], regularizer=0.02, learning_rate=0.02</t>
         </is>
       </c>
     </row>

</xml_diff>